<commit_message>
Ran the friedman test along with the post hocs.
</commit_message>
<xml_diff>
--- a/Play Exp 3 (Reinforcer) Data MASTER2.xlsx
+++ b/Play Exp 3 (Reinforcer) Data MASTER2.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jettvernaci/Desktop/SP20/Consulting/Mehrkam Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B536FB-03BF-D24A-AB0F-5DDDD5F01A2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D613A0-8C99-9E4E-8596-59AA19A885FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Averages" sheetId="11" r:id="rId1"/>
     <sheet name="Master Reinforcer" sheetId="14" r:id="rId2"/>
-    <sheet name="P1_Kobe&amp;Ian" sheetId="1" r:id="rId3"/>
-    <sheet name="P2_Sally&amp;Vanya" sheetId="2" r:id="rId4"/>
-    <sheet name="P3_Rocky&amp;Oaky" sheetId="3" r:id="rId5"/>
-    <sheet name="P4_Rosie&amp;Carlie" sheetId="5" r:id="rId6"/>
-    <sheet name="P5_Jude&amp;Luna" sheetId="4" r:id="rId7"/>
-    <sheet name="P6_Kodi &amp; Kaia" sheetId="6" r:id="rId8"/>
-    <sheet name="P7_Dax &amp; Fiona" sheetId="7" r:id="rId9"/>
-    <sheet name="P8_Misha&amp;Houston" sheetId="8" r:id="rId10"/>
-    <sheet name="P9_Gunner&amp;Cato" sheetId="9" r:id="rId11"/>
-    <sheet name="P10_Coffee&amp;Mason" sheetId="10" r:id="rId12"/>
-    <sheet name="P11_Rev&amp;Blitz" sheetId="12" r:id="rId13"/>
-    <sheet name="P12_Magnum&amp;Toby" sheetId="13" r:id="rId14"/>
+    <sheet name="Master Averages" sheetId="15" r:id="rId3"/>
+    <sheet name="P1_Kobe&amp;Ian" sheetId="1" r:id="rId4"/>
+    <sheet name="P2_Sally&amp;Vanya" sheetId="2" r:id="rId5"/>
+    <sheet name="P3_Rocky&amp;Oaky" sheetId="3" r:id="rId6"/>
+    <sheet name="P4_Rosie&amp;Carlie" sheetId="5" r:id="rId7"/>
+    <sheet name="P5_Jude&amp;Luna" sheetId="4" r:id="rId8"/>
+    <sheet name="P6_Kodi &amp; Kaia" sheetId="6" r:id="rId9"/>
+    <sheet name="P7_Dax &amp; Fiona" sheetId="7" r:id="rId10"/>
+    <sheet name="P8_Misha&amp;Houston" sheetId="8" r:id="rId11"/>
+    <sheet name="P9_Gunner&amp;Cato" sheetId="9" r:id="rId12"/>
+    <sheet name="P10_Coffee&amp;Mason" sheetId="10" r:id="rId13"/>
+    <sheet name="P11_Rev&amp;Blitz" sheetId="12" r:id="rId14"/>
+    <sheet name="P12_Magnum&amp;Toby" sheetId="13" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="63">
   <si>
     <t>Session</t>
   </si>
@@ -232,6 +233,9 @@
   </si>
   <si>
     <t>Sample #</t>
+  </si>
+  <si>
+    <t>Average PlayTime (Sec)</t>
   </si>
 </sst>
 </file>
@@ -9676,6 +9680,286 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="3"/>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>120+36+6</f>
+        <v>162</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="3"/>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <f>240+27</f>
+        <v>267</v>
+      </c>
+      <c r="D3">
+        <f>95</f>
+        <v>95</v>
+      </c>
+      <c r="E3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="3"/>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <f>180+40+4</f>
+        <v>224</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2"/>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <f>180+57</f>
+        <v>237</v>
+      </c>
+      <c r="D5">
+        <f>120+17</f>
+        <v>137</v>
+      </c>
+      <c r="E5">
+        <f>180+2</f>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2"/>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <f>120+1+7</f>
+        <v>128</v>
+      </c>
+      <c r="D6">
+        <f>60+51+6</f>
+        <v>117</v>
+      </c>
+      <c r="E6">
+        <f>120+55</f>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2"/>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <f>180+27</f>
+        <v>207</v>
+      </c>
+      <c r="D7">
+        <f>120+3</f>
+        <v>123</v>
+      </c>
+      <c r="E7">
+        <f>180+44</f>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8">
+        <f>SUM(C2:C7)</f>
+        <v>1225</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ref="D8:E8" si="0">SUM(D2:D7)</f>
+        <v>480</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>634</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9">
+        <f>AVERAGE(C2:C7)</f>
+        <v>204.16666666666666</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ref="D9:E9" si="1">AVERAGE(D2:D7)</f>
+        <v>80</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>105.66666666666667</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10">
+        <f>STDEV(C2:C7)</f>
+        <v>51.003594644560778</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ref="D10:E10" si="2">STDEV(D2:D7)</f>
+        <v>60.4582500573743</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>99.740997922953767</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11">
+        <f>C10/SQRT(6)</f>
+        <v>20.822130321153779</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ref="D11:E11" si="3">D10/SQRT(6)</f>
+        <v>24.681977230359809</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="3"/>
+        <v>40.719091891205593</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="C16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17">
+        <v>1225</v>
+      </c>
+      <c r="D17">
+        <v>480</v>
+      </c>
+      <c r="E17">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18">
+        <v>204.16666666666666</v>
+      </c>
+      <c r="D18">
+        <v>80</v>
+      </c>
+      <c r="E18">
+        <v>105.66666666666667</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19">
+        <v>51.003594644560778</v>
+      </c>
+      <c r="D19">
+        <v>60.4582500573743</v>
+      </c>
+      <c r="E19">
+        <v>99.740997922953767</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20">
+        <v>20.822130321153779</v>
+      </c>
+      <c r="D20">
+        <v>24.681977230359809</v>
+      </c>
+      <c r="E20">
+        <v>40.719091891205593</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -9890,7 +10174,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -10090,7 +10374,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -10443,7 +10727,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -10643,7 +10927,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -10667,10 +10951,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:F157"/>
+  <dimension ref="A1:F145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -10747,7 +11031,7 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B67" si="0">B3+1</f>
+        <f t="shared" ref="B4:B37" si="0">B3+1</f>
         <v>3</v>
       </c>
       <c r="C4">
@@ -11460,14 +11744,14 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="B38">
-        <f t="shared" si="0"/>
+        <f>B37+1</f>
         <v>37</v>
       </c>
       <c r="C38">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D38" s="4">
         <v>1</v>
@@ -11476,20 +11760,19 @@
         <v>1</v>
       </c>
       <c r="F38" s="4">
-        <f>91+15</f>
-        <v>106</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="B39">
-        <f t="shared" si="0"/>
+        <f>B38+1</f>
         <v>38</v>
       </c>
       <c r="C39">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D39" s="4">
         <v>2</v>
@@ -11498,20 +11781,19 @@
         <v>1</v>
       </c>
       <c r="F39" s="4">
-        <f>210+13</f>
-        <v>223</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="B40">
-        <f t="shared" si="0"/>
+        <f>B39+1</f>
         <v>39</v>
       </c>
       <c r="C40">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D40" s="4">
         <v>3</v>
@@ -11520,20 +11802,19 @@
         <v>1</v>
       </c>
       <c r="F40" s="4">
-        <f>180+24+8</f>
-        <v>212</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="B41">
-        <f t="shared" si="0"/>
+        <f>B40+1</f>
         <v>40</v>
       </c>
       <c r="C41">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D41" s="4">
         <v>4</v>
@@ -11542,7 +11823,7 @@
         <v>1</v>
       </c>
       <c r="F41" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -11550,20 +11831,20 @@
         <v>34</v>
       </c>
       <c r="B42">
-        <f t="shared" si="0"/>
+        <f>B41+1</f>
         <v>41</v>
       </c>
       <c r="C42">
         <v>10</v>
       </c>
       <c r="D42" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E42" s="4">
         <v>1</v>
       </c>
       <c r="F42" s="4">
-        <v>7</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -11571,104 +11852,104 @@
         <v>34</v>
       </c>
       <c r="B43">
-        <f t="shared" si="0"/>
+        <f>B42+1</f>
         <v>42</v>
       </c>
       <c r="C43">
         <v>10</v>
       </c>
       <c r="D43" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E43" s="4">
         <v>1</v>
       </c>
       <c r="F43" s="4">
-        <v>30</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B44">
-        <f t="shared" si="0"/>
+        <f>B43+1</f>
         <v>43</v>
       </c>
       <c r="C44">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D44" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E44" s="4">
         <v>1</v>
       </c>
       <c r="F44" s="4">
-        <v>4</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B45">
-        <f t="shared" si="0"/>
+        <f>B44+1</f>
         <v>44</v>
       </c>
       <c r="C45">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D45" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E45" s="4">
         <v>1</v>
       </c>
       <c r="F45" s="4">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B46">
-        <f t="shared" si="0"/>
+        <f>B45+1</f>
         <v>45</v>
       </c>
       <c r="C46">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D46" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E46" s="4">
         <v>1</v>
       </c>
       <c r="F46" s="4">
-        <v>94</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B47">
-        <f t="shared" si="0"/>
+        <f>B46+1</f>
         <v>46</v>
       </c>
       <c r="C47">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D47" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E47" s="4">
         <v>1</v>
       </c>
       <c r="F47" s="4">
-        <v>113</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -11676,20 +11957,20 @@
         <v>35</v>
       </c>
       <c r="B48">
-        <f t="shared" si="0"/>
+        <f>B47+1</f>
         <v>47</v>
       </c>
       <c r="C48">
         <v>11</v>
       </c>
       <c r="D48" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E48" s="4">
         <v>1</v>
       </c>
       <c r="F48" s="4">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -11697,38 +11978,38 @@
         <v>35</v>
       </c>
       <c r="B49">
-        <f t="shared" si="0"/>
+        <f>B48+1</f>
         <v>48</v>
       </c>
       <c r="C49">
         <v>11</v>
       </c>
       <c r="D49" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E49" s="4">
         <v>1</v>
       </c>
       <c r="F49" s="4">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="B50">
-        <f t="shared" si="0"/>
+        <f>B49+1</f>
         <v>49</v>
       </c>
       <c r="C50">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D50" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E50" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F50" s="4">
         <v>0</v>
@@ -11736,65 +12017,65 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="B51">
-        <f t="shared" si="0"/>
+        <f>B50+1</f>
         <v>50</v>
       </c>
       <c r="C51">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D51" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E51" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F51" s="4">
-        <v>81</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="B52">
-        <f t="shared" si="0"/>
+        <f>B51+1</f>
         <v>51</v>
       </c>
       <c r="C52">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D52" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E52" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F52" s="4">
-        <v>54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="B53">
-        <f t="shared" si="0"/>
+        <f>B52+1</f>
         <v>52</v>
       </c>
       <c r="C53">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D53" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E53" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F53" s="4">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -11802,14 +12083,14 @@
         <v>10</v>
       </c>
       <c r="B54">
-        <f t="shared" si="0"/>
+        <f>B53+1</f>
         <v>53</v>
       </c>
       <c r="C54">
         <v>2</v>
       </c>
       <c r="D54" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E54" s="4">
         <v>2</v>
@@ -11823,14 +12104,14 @@
         <v>10</v>
       </c>
       <c r="B55">
-        <f t="shared" si="0"/>
+        <f>B54+1</f>
         <v>54</v>
       </c>
       <c r="C55">
         <v>2</v>
       </c>
       <c r="D55" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E55" s="4">
         <v>2</v>
@@ -11841,17 +12122,17 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B56">
-        <f t="shared" si="0"/>
+        <f>B55+1</f>
         <v>55</v>
       </c>
       <c r="C56">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D56" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E56" s="4">
         <v>2</v>
@@ -11862,17 +12143,17 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B57">
-        <f t="shared" si="0"/>
+        <f>B56+1</f>
         <v>56</v>
       </c>
       <c r="C57">
+        <v>3</v>
+      </c>
+      <c r="D57" s="4">
         <v>2</v>
-      </c>
-      <c r="D57" s="4">
-        <v>4</v>
       </c>
       <c r="E57" s="4">
         <v>2</v>
@@ -11883,17 +12164,17 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B58">
-        <f t="shared" si="0"/>
+        <f>B57+1</f>
         <v>57</v>
       </c>
       <c r="C58">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D58" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E58" s="4">
         <v>2</v>
@@ -11904,23 +12185,23 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B59">
-        <f t="shared" si="0"/>
+        <f>B58+1</f>
         <v>58</v>
       </c>
       <c r="C59">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D59" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E59" s="4">
         <v>2</v>
       </c>
       <c r="F59" s="4">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -11928,14 +12209,14 @@
         <v>11</v>
       </c>
       <c r="B60">
-        <f t="shared" si="0"/>
+        <f>B59+1</f>
         <v>59</v>
       </c>
       <c r="C60">
         <v>3</v>
       </c>
       <c r="D60" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E60" s="4">
         <v>2</v>
@@ -11949,14 +12230,14 @@
         <v>11</v>
       </c>
       <c r="B61">
-        <f t="shared" si="0"/>
+        <f>B60+1</f>
         <v>60</v>
       </c>
       <c r="C61">
         <v>3</v>
       </c>
       <c r="D61" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E61" s="4">
         <v>2</v>
@@ -11967,17 +12248,17 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B62">
-        <f t="shared" si="0"/>
+        <f>B61+1</f>
         <v>61</v>
       </c>
       <c r="C62">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D62" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E62" s="4">
         <v>2</v>
@@ -11988,38 +12269,38 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B63">
-        <f t="shared" si="0"/>
+        <f>B62+1</f>
         <v>62</v>
       </c>
       <c r="C63">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D63" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E63" s="4">
         <v>2</v>
       </c>
       <c r="F63" s="4">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B64">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B64:B85" si="1">B63+1</f>
         <v>63</v>
       </c>
       <c r="C64">
+        <v>4</v>
+      </c>
+      <c r="D64" s="4">
         <v>3</v>
-      </c>
-      <c r="D64" s="4">
-        <v>5</v>
       </c>
       <c r="E64" s="4">
         <v>2</v>
@@ -12030,17 +12311,17 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>64</v>
       </c>
       <c r="C65">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D65" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E65" s="4">
         <v>2</v>
@@ -12054,14 +12335,14 @@
         <v>12</v>
       </c>
       <c r="B66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>65</v>
       </c>
       <c r="C66">
         <v>4</v>
       </c>
       <c r="D66" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E66" s="4">
         <v>2</v>
@@ -12075,14 +12356,14 @@
         <v>12</v>
       </c>
       <c r="B67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>66</v>
       </c>
       <c r="C67">
         <v>4</v>
       </c>
       <c r="D67" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E67" s="4">
         <v>2</v>
@@ -12093,17 +12374,17 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B68">
-        <f t="shared" ref="B68:B131" si="1">B67+1</f>
+        <f t="shared" si="1"/>
         <v>67</v>
       </c>
       <c r="C68">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D68" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E68" s="4">
         <v>2</v>
@@ -12114,17 +12395,17 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B69">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
       <c r="C69">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D69" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E69" s="4">
         <v>2</v>
@@ -12135,17 +12416,17 @@
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B70">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
       <c r="C70">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D70" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E70" s="4">
         <v>2</v>
@@ -12156,17 +12437,17 @@
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B71">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="C71">
+        <v>6</v>
+      </c>
+      <c r="D71" s="4">
         <v>4</v>
-      </c>
-      <c r="D71" s="4">
-        <v>6</v>
       </c>
       <c r="E71" s="4">
         <v>2</v>
@@ -12187,7 +12468,7 @@
         <v>6</v>
       </c>
       <c r="D72" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E72" s="4">
         <v>2</v>
@@ -12208,7 +12489,7 @@
         <v>6</v>
       </c>
       <c r="D73" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E73" s="4">
         <v>2</v>
@@ -12219,17 +12500,17 @@
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B74">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
       <c r="C74">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D74" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E74" s="4">
         <v>2</v>
@@ -12240,65 +12521,65 @@
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B75">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
       <c r="C75">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D75" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E75" s="4">
         <v>2</v>
       </c>
       <c r="F75" s="4">
-        <v>0</v>
+        <v>95</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B76">
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
       <c r="C76">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D76" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E76" s="4">
         <v>2</v>
       </c>
       <c r="F76" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B77">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
       <c r="C77">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D77" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E77" s="4">
         <v>2</v>
       </c>
       <c r="F77" s="4">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -12313,13 +12594,13 @@
         <v>7</v>
       </c>
       <c r="D78" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E78" s="4">
         <v>2</v>
       </c>
       <c r="F78" s="4">
-        <v>0</v>
+        <v>117</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -12334,97 +12615,99 @@
         <v>7</v>
       </c>
       <c r="D79" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E79" s="4">
         <v>2</v>
       </c>
       <c r="F79" s="4">
-        <v>95</v>
+        <v>123</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="B80">
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
       <c r="C80">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D80" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E80" s="4">
         <v>2</v>
       </c>
       <c r="F80" s="4">
-        <v>8</v>
+        <f>77+5.5</f>
+        <v>82.5</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="B81">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="C81">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D81" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E81" s="4">
         <v>2</v>
       </c>
       <c r="F81" s="4">
-        <v>137</v>
+        <f>43+11</f>
+        <v>54</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="B82">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
       <c r="C82">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D82" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E82" s="4">
         <v>2</v>
       </c>
       <c r="F82" s="4">
-        <v>117</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="B83">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
       <c r="C83">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D83" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E83" s="4">
         <v>2</v>
       </c>
       <c r="F83" s="4">
-        <v>123</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -12439,14 +12722,13 @@
         <v>8</v>
       </c>
       <c r="D84" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E84" s="4">
         <v>2</v>
       </c>
       <c r="F84" s="4">
-        <f>77+5.5</f>
-        <v>82.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -12461,29 +12743,28 @@
         <v>8</v>
       </c>
       <c r="D85" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E85" s="4">
         <v>2</v>
       </c>
       <c r="F85" s="4">
-        <f>43+11</f>
-        <v>54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B86">
-        <f t="shared" si="1"/>
+        <f>B85+1</f>
         <v>85</v>
       </c>
       <c r="C86">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D86" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E86" s="4">
         <v>2</v>
@@ -12494,17 +12775,17 @@
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B87">
-        <f t="shared" si="1"/>
+        <f>B86+1</f>
         <v>86</v>
       </c>
       <c r="C87">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D87" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E87" s="4">
         <v>2</v>
@@ -12515,38 +12796,38 @@
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B88">
-        <f t="shared" si="1"/>
+        <f>B87+1</f>
         <v>87</v>
       </c>
       <c r="C88">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D88" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E88" s="4">
         <v>2</v>
       </c>
       <c r="F88" s="4">
-        <v>0</v>
+        <v>43</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B89">
-        <f t="shared" si="1"/>
+        <f>B88+1</f>
         <v>88</v>
       </c>
       <c r="C89">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D89" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E89" s="4">
         <v>2</v>
@@ -12557,17 +12838,17 @@
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="B90">
-        <f t="shared" si="1"/>
+        <f>B89+1</f>
         <v>89</v>
       </c>
       <c r="C90">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D90" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E90" s="4">
         <v>2</v>
@@ -12578,17 +12859,17 @@
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="B91">
-        <f t="shared" si="1"/>
+        <f>B90+1</f>
         <v>90</v>
       </c>
       <c r="C91">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D91" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E91" s="4">
         <v>2</v>
@@ -12599,59 +12880,59 @@
     </row>
     <row r="92" spans="1:6">
       <c r="A92" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="B92">
-        <f t="shared" si="1"/>
+        <f>B91+1</f>
         <v>91</v>
       </c>
       <c r="C92">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D92" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E92" s="4">
         <v>2</v>
       </c>
       <c r="F92" s="4">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="B93">
-        <f t="shared" si="1"/>
+        <f>B92+1</f>
         <v>92</v>
       </c>
       <c r="C93">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D93" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E93" s="4">
         <v>2</v>
       </c>
       <c r="F93" s="4">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B94">
-        <f t="shared" si="1"/>
+        <f>B93+1</f>
         <v>93</v>
       </c>
       <c r="C94">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D94" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E94" s="4">
         <v>2</v>
@@ -12662,83 +12943,83 @@
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B95">
-        <f t="shared" si="1"/>
+        <f>B94+1</f>
         <v>94</v>
       </c>
       <c r="C95">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D95" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E95" s="4">
         <v>2</v>
       </c>
       <c r="F95" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B96">
-        <f t="shared" si="1"/>
+        <f>B95+1</f>
         <v>95</v>
       </c>
       <c r="C96">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D96" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E96" s="4">
         <v>2</v>
       </c>
       <c r="F96" s="4">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B97">
-        <f t="shared" si="1"/>
+        <f>B96+1</f>
         <v>96</v>
       </c>
       <c r="C97">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D97" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E97" s="4">
         <v>2</v>
       </c>
       <c r="F97" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="98" spans="1:6">
       <c r="A98" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B98">
-        <f t="shared" si="1"/>
+        <f>B97+1</f>
         <v>97</v>
       </c>
       <c r="C98">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D98" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E98" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F98" s="4">
         <v>0</v>
@@ -12746,20 +13027,20 @@
     </row>
     <row r="99" spans="1:6">
       <c r="A99" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B99">
-        <f t="shared" si="1"/>
+        <f>B98+1</f>
         <v>98</v>
       </c>
       <c r="C99">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D99" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E99" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F99" s="4">
         <v>0</v>
@@ -12767,62 +13048,62 @@
     </row>
     <row r="100" spans="1:6">
       <c r="A100" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="B100">
-        <f t="shared" si="1"/>
+        <f>B99+1</f>
         <v>99</v>
       </c>
       <c r="C100">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D100" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E100" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F100" s="4">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c r="A101" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="B101">
-        <f t="shared" si="1"/>
+        <f>B100+1</f>
         <v>100</v>
       </c>
       <c r="C101">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D101" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E101" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F101" s="4">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:6">
       <c r="A102" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="B102">
-        <f t="shared" si="1"/>
+        <f>B101+1</f>
         <v>101</v>
       </c>
       <c r="C102">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D102" s="4">
+        <v>5</v>
+      </c>
+      <c r="E102" s="4">
         <v>3</v>
-      </c>
-      <c r="E102" s="4">
-        <v>2</v>
       </c>
       <c r="F102" s="4">
         <v>0</v>
@@ -12830,80 +13111,80 @@
     </row>
     <row r="103" spans="1:6">
       <c r="A103" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="B103">
-        <f t="shared" si="1"/>
+        <f>B102+1</f>
         <v>102</v>
       </c>
       <c r="C103">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D103" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E103" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F103" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B104">
-        <f t="shared" si="1"/>
+        <f>B103+1</f>
         <v>103</v>
       </c>
       <c r="C104">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D104" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E104" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F104" s="4">
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B105">
-        <f t="shared" si="1"/>
+        <f>B104+1</f>
         <v>104</v>
       </c>
       <c r="C105">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D105" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E105" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F105" s="4">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B106">
-        <f t="shared" si="1"/>
+        <f>B105+1</f>
         <v>105</v>
       </c>
       <c r="C106">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D106" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E106" s="4">
         <v>3</v>
@@ -12914,17 +13195,17 @@
     </row>
     <row r="107" spans="1:6">
       <c r="A107" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B107">
-        <f t="shared" si="1"/>
+        <f>B106+1</f>
         <v>106</v>
       </c>
       <c r="C107">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D107" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E107" s="4">
         <v>3</v>
@@ -12935,17 +13216,17 @@
     </row>
     <row r="108" spans="1:6">
       <c r="A108" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B108">
-        <f t="shared" si="1"/>
+        <f>B107+1</f>
         <v>107</v>
       </c>
       <c r="C108">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D108" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E108" s="4">
         <v>3</v>
@@ -12956,17 +13237,17 @@
     </row>
     <row r="109" spans="1:6">
       <c r="A109" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B109">
-        <f t="shared" si="1"/>
+        <f>B108+1</f>
         <v>108</v>
       </c>
       <c r="C109">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D109" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E109" s="4">
         <v>3</v>
@@ -12977,17 +13258,17 @@
     </row>
     <row r="110" spans="1:6">
       <c r="A110" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B110">
-        <f t="shared" si="1"/>
+        <f>B109+1</f>
         <v>109</v>
       </c>
       <c r="C110">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D110" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E110" s="4">
         <v>3</v>
@@ -12998,17 +13279,17 @@
     </row>
     <row r="111" spans="1:6">
       <c r="A111" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B111">
-        <f t="shared" si="1"/>
+        <f>B110+1</f>
         <v>110</v>
       </c>
       <c r="C111">
+        <v>4</v>
+      </c>
+      <c r="D111" s="4">
         <v>2</v>
-      </c>
-      <c r="D111" s="4">
-        <v>6</v>
       </c>
       <c r="E111" s="4">
         <v>3</v>
@@ -13019,17 +13300,17 @@
     </row>
     <row r="112" spans="1:6">
       <c r="A112" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B112">
-        <f t="shared" si="1"/>
+        <f>B111+1</f>
         <v>111</v>
       </c>
       <c r="C112">
+        <v>4</v>
+      </c>
+      <c r="D112" s="4">
         <v>3</v>
-      </c>
-      <c r="D112" s="4">
-        <v>1</v>
       </c>
       <c r="E112" s="4">
         <v>3</v>
@@ -13040,17 +13321,17 @@
     </row>
     <row r="113" spans="1:6">
       <c r="A113" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B113">
-        <f t="shared" si="1"/>
+        <f>B112+1</f>
         <v>112</v>
       </c>
       <c r="C113">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D113" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E113" s="4">
         <v>3</v>
@@ -13061,17 +13342,17 @@
     </row>
     <row r="114" spans="1:6">
       <c r="A114" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B114">
-        <f t="shared" si="1"/>
+        <f>B113+1</f>
         <v>113</v>
       </c>
       <c r="C114">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D114" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E114" s="4">
         <v>3</v>
@@ -13082,17 +13363,17 @@
     </row>
     <row r="115" spans="1:6">
       <c r="A115" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B115">
-        <f t="shared" si="1"/>
+        <f>B114+1</f>
         <v>114</v>
       </c>
       <c r="C115">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D115" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E115" s="4">
         <v>3</v>
@@ -13103,17 +13384,17 @@
     </row>
     <row r="116" spans="1:6">
       <c r="A116" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B116">
-        <f t="shared" si="1"/>
+        <f>B115+1</f>
         <v>115</v>
       </c>
       <c r="C116">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D116" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E116" s="4">
         <v>3</v>
@@ -13124,17 +13405,17 @@
     </row>
     <row r="117" spans="1:6">
       <c r="A117" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B117">
-        <f t="shared" si="1"/>
+        <f>B116+1</f>
         <v>116</v>
       </c>
       <c r="C117">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D117" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E117" s="4">
         <v>3</v>
@@ -13145,17 +13426,17 @@
     </row>
     <row r="118" spans="1:6">
       <c r="A118" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B118">
-        <f t="shared" si="1"/>
+        <f>B117+1</f>
         <v>117</v>
       </c>
       <c r="C118">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D118" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E118" s="4">
         <v>3</v>
@@ -13166,17 +13447,17 @@
     </row>
     <row r="119" spans="1:6">
       <c r="A119" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B119">
-        <f t="shared" si="1"/>
+        <f>B118+1</f>
         <v>118</v>
       </c>
       <c r="C119">
+        <v>6</v>
+      </c>
+      <c r="D119" s="4">
         <v>4</v>
-      </c>
-      <c r="D119" s="4">
-        <v>2</v>
       </c>
       <c r="E119" s="4">
         <v>3</v>
@@ -13187,17 +13468,17 @@
     </row>
     <row r="120" spans="1:6">
       <c r="A120" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B120">
-        <f t="shared" si="1"/>
+        <f>B119+1</f>
         <v>119</v>
       </c>
       <c r="C120">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D120" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E120" s="4">
         <v>3</v>
@@ -13208,17 +13489,17 @@
     </row>
     <row r="121" spans="1:6">
       <c r="A121" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B121">
-        <f t="shared" si="1"/>
+        <f>B120+1</f>
         <v>120</v>
       </c>
       <c r="C121">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D121" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E121" s="4">
         <v>3</v>
@@ -13229,17 +13510,17 @@
     </row>
     <row r="122" spans="1:6">
       <c r="A122" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B122">
-        <f t="shared" si="1"/>
+        <f>B121+1</f>
         <v>121</v>
       </c>
       <c r="C122">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D122" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E122" s="4">
         <v>3</v>
@@ -13250,38 +13531,38 @@
     </row>
     <row r="123" spans="1:6">
       <c r="A123" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B123">
-        <f t="shared" si="1"/>
+        <f>B122+1</f>
         <v>122</v>
       </c>
       <c r="C123">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D123" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E123" s="4">
         <v>3</v>
       </c>
       <c r="F123" s="4">
-        <v>0</v>
+        <v>53</v>
       </c>
     </row>
     <row r="124" spans="1:6">
       <c r="A124" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B124">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="B124:B149" si="2">B123+1</f>
         <v>123</v>
       </c>
       <c r="C124">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D124" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E124" s="4">
         <v>3</v>
@@ -13292,80 +13573,80 @@
     </row>
     <row r="125" spans="1:6">
       <c r="A125" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B125">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>124</v>
       </c>
       <c r="C125">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D125" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E125" s="4">
         <v>3</v>
       </c>
       <c r="F125" s="4">
-        <v>0</v>
+        <v>182</v>
       </c>
     </row>
     <row r="126" spans="1:6">
       <c r="A126" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B126">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>125</v>
       </c>
       <c r="C126">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D126" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E126" s="4">
         <v>3</v>
       </c>
       <c r="F126" s="4">
-        <v>0</v>
+        <v>175</v>
       </c>
     </row>
     <row r="127" spans="1:6">
       <c r="A127" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B127">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>126</v>
       </c>
       <c r="C127">
+        <v>7</v>
+      </c>
+      <c r="D127" s="4">
         <v>6</v>
-      </c>
-      <c r="D127" s="4">
-        <v>4</v>
       </c>
       <c r="E127" s="4">
         <v>3</v>
       </c>
       <c r="F127" s="4">
-        <v>0</v>
+        <v>224</v>
       </c>
     </row>
     <row r="128" spans="1:6">
       <c r="A128" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="B128">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>127</v>
       </c>
       <c r="C128">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D128" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E128" s="4">
         <v>3</v>
@@ -13376,17 +13657,17 @@
     </row>
     <row r="129" spans="1:6">
       <c r="A129" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="B129">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>128</v>
       </c>
       <c r="C129">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D129" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E129" s="4">
         <v>3</v>
@@ -13397,17 +13678,17 @@
     </row>
     <row r="130" spans="1:6">
       <c r="A130" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="B130">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>129</v>
       </c>
       <c r="C130">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D130" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E130" s="4">
         <v>3</v>
@@ -13418,122 +13699,123 @@
     </row>
     <row r="131" spans="1:6">
       <c r="A131" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="B131">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>130</v>
       </c>
       <c r="C131">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D131" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E131" s="4">
         <v>3</v>
       </c>
       <c r="F131" s="4">
-        <v>53</v>
+        <v>106</v>
       </c>
     </row>
     <row r="132" spans="1:6">
       <c r="A132" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="B132">
-        <f t="shared" ref="B132:B157" si="2">B131+1</f>
+        <f t="shared" si="2"/>
         <v>131</v>
       </c>
       <c r="C132">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D132" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E132" s="4">
         <v>3</v>
       </c>
       <c r="F132" s="4">
-        <v>0</v>
+        <f>128+2.5</f>
+        <v>130.5</v>
       </c>
     </row>
     <row r="133" spans="1:6">
       <c r="A133" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="B133">
         <f t="shared" si="2"/>
         <v>132</v>
       </c>
       <c r="C133">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D133" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E133" s="4">
         <v>3</v>
       </c>
       <c r="F133" s="4">
-        <v>182</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:6">
       <c r="A134" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B134">
-        <f t="shared" si="2"/>
+        <f>B133+1</f>
         <v>133</v>
       </c>
       <c r="C134">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D134" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E134" s="4">
         <v>3</v>
       </c>
       <c r="F134" s="4">
-        <v>175</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:6">
       <c r="A135" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B135">
-        <f t="shared" si="2"/>
+        <f>B134+1</f>
         <v>134</v>
       </c>
       <c r="C135">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D135" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E135" s="4">
         <v>3</v>
       </c>
       <c r="F135" s="4">
-        <v>224</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:6">
       <c r="A136" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B136">
-        <f t="shared" si="2"/>
+        <f>B135+1</f>
         <v>135</v>
       </c>
       <c r="C136">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D136" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E136" s="4">
         <v>3</v>
@@ -13544,17 +13826,17 @@
     </row>
     <row r="137" spans="1:6">
       <c r="A137" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B137">
-        <f t="shared" si="2"/>
+        <f>B136+1</f>
         <v>136</v>
       </c>
       <c r="C137">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D137" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E137" s="4">
         <v>3</v>
@@ -13565,17 +13847,17 @@
     </row>
     <row r="138" spans="1:6">
       <c r="A138" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B138">
-        <f t="shared" si="2"/>
+        <f>B137+1</f>
         <v>137</v>
       </c>
       <c r="C138">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D138" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E138" s="4">
         <v>3</v>
@@ -13586,60 +13868,59 @@
     </row>
     <row r="139" spans="1:6">
       <c r="A139" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B139">
-        <f t="shared" si="2"/>
+        <f>B138+1</f>
         <v>138</v>
       </c>
       <c r="C139">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D139" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E139" s="4">
         <v>3</v>
       </c>
       <c r="F139" s="4">
-        <v>106</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:6">
       <c r="A140" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="B140">
-        <f t="shared" si="2"/>
+        <f>B139+1</f>
         <v>139</v>
       </c>
       <c r="C140">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D140" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E140" s="4">
         <v>3</v>
       </c>
       <c r="F140" s="4">
-        <f>128+2.5</f>
-        <v>130.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:6">
       <c r="A141" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="B141">
-        <f t="shared" si="2"/>
+        <f>B140+1</f>
         <v>140</v>
       </c>
       <c r="C141">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D141" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E141" s="4">
         <v>3</v>
@@ -13650,60 +13931,59 @@
     </row>
     <row r="142" spans="1:6">
       <c r="A142" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="B142">
-        <f t="shared" si="2"/>
+        <f>B141+1</f>
         <v>141</v>
       </c>
       <c r="C142">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D142" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E142" s="4">
         <v>3</v>
       </c>
       <c r="F142" s="4">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:6">
       <c r="A143" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="B143">
-        <f t="shared" si="2"/>
+        <f>B142+1</f>
         <v>142</v>
       </c>
       <c r="C143">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D143" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E143" s="4">
         <v>3</v>
       </c>
       <c r="F143" s="4">
-        <f>48+120</f>
-        <v>168</v>
+        <v>35</v>
       </c>
     </row>
     <row r="144" spans="1:6">
       <c r="A144" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="B144">
-        <f t="shared" si="2"/>
+        <f>B143+1</f>
         <v>143</v>
       </c>
       <c r="C144">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D144" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E144" s="4">
         <v>3</v>
@@ -13714,274 +13994,22 @@
     </row>
     <row r="145" spans="1:6">
       <c r="A145" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="B145">
-        <f t="shared" si="2"/>
+        <f>B144+1</f>
         <v>144</v>
       </c>
       <c r="C145">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D145" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E145" s="4">
         <v>3</v>
       </c>
       <c r="F145" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6">
-      <c r="A146" t="s">
-        <v>34</v>
-      </c>
-      <c r="B146">
-        <f t="shared" si="2"/>
-        <v>145</v>
-      </c>
-      <c r="C146">
-        <v>10</v>
-      </c>
-      <c r="D146" s="4">
-        <v>1</v>
-      </c>
-      <c r="E146" s="4">
-        <v>3</v>
-      </c>
-      <c r="F146" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6">
-      <c r="A147" t="s">
-        <v>34</v>
-      </c>
-      <c r="B147">
-        <f t="shared" si="2"/>
-        <v>146</v>
-      </c>
-      <c r="C147">
-        <v>10</v>
-      </c>
-      <c r="D147" s="4">
-        <v>2</v>
-      </c>
-      <c r="E147" s="4">
-        <v>3</v>
-      </c>
-      <c r="F147" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6">
-      <c r="A148" t="s">
-        <v>34</v>
-      </c>
-      <c r="B148">
-        <f t="shared" si="2"/>
-        <v>147</v>
-      </c>
-      <c r="C148">
-        <v>10</v>
-      </c>
-      <c r="D148" s="4">
-        <v>3</v>
-      </c>
-      <c r="E148" s="4">
-        <v>3</v>
-      </c>
-      <c r="F148" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6">
-      <c r="A149" t="s">
-        <v>34</v>
-      </c>
-      <c r="B149">
-        <f t="shared" si="2"/>
-        <v>148</v>
-      </c>
-      <c r="C149">
-        <v>10</v>
-      </c>
-      <c r="D149" s="4">
-        <v>4</v>
-      </c>
-      <c r="E149" s="4">
-        <v>3</v>
-      </c>
-      <c r="F149" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6">
-      <c r="A150" t="s">
-        <v>34</v>
-      </c>
-      <c r="B150">
-        <f t="shared" si="2"/>
-        <v>149</v>
-      </c>
-      <c r="C150">
-        <v>10</v>
-      </c>
-      <c r="D150" s="4">
-        <v>5</v>
-      </c>
-      <c r="E150" s="4">
-        <v>3</v>
-      </c>
-      <c r="F150" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6">
-      <c r="A151" t="s">
-        <v>34</v>
-      </c>
-      <c r="B151">
-        <f t="shared" si="2"/>
-        <v>150</v>
-      </c>
-      <c r="C151">
-        <v>10</v>
-      </c>
-      <c r="D151" s="4">
-        <v>6</v>
-      </c>
-      <c r="E151" s="4">
-        <v>3</v>
-      </c>
-      <c r="F151" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6">
-      <c r="A152" t="s">
-        <v>35</v>
-      </c>
-      <c r="B152">
-        <f t="shared" si="2"/>
-        <v>151</v>
-      </c>
-      <c r="C152">
-        <v>11</v>
-      </c>
-      <c r="D152" s="4">
-        <v>1</v>
-      </c>
-      <c r="E152" s="4">
-        <v>3</v>
-      </c>
-      <c r="F152" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6">
-      <c r="A153" t="s">
-        <v>35</v>
-      </c>
-      <c r="B153">
-        <f t="shared" si="2"/>
-        <v>152</v>
-      </c>
-      <c r="C153">
-        <v>11</v>
-      </c>
-      <c r="D153" s="4">
-        <v>2</v>
-      </c>
-      <c r="E153" s="4">
-        <v>3</v>
-      </c>
-      <c r="F153" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6">
-      <c r="A154" t="s">
-        <v>35</v>
-      </c>
-      <c r="B154">
-        <f t="shared" si="2"/>
-        <v>153</v>
-      </c>
-      <c r="C154">
-        <v>11</v>
-      </c>
-      <c r="D154" s="4">
-        <v>3</v>
-      </c>
-      <c r="E154" s="4">
-        <v>3</v>
-      </c>
-      <c r="F154" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6">
-      <c r="A155" t="s">
-        <v>35</v>
-      </c>
-      <c r="B155">
-        <f t="shared" si="2"/>
-        <v>154</v>
-      </c>
-      <c r="C155">
-        <v>11</v>
-      </c>
-      <c r="D155" s="4">
-        <v>4</v>
-      </c>
-      <c r="E155" s="4">
-        <v>3</v>
-      </c>
-      <c r="F155" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6">
-      <c r="A156" t="s">
-        <v>35</v>
-      </c>
-      <c r="B156">
-        <f t="shared" si="2"/>
-        <v>155</v>
-      </c>
-      <c r="C156">
-        <v>11</v>
-      </c>
-      <c r="D156" s="4">
-        <v>5</v>
-      </c>
-      <c r="E156" s="4">
-        <v>3</v>
-      </c>
-      <c r="F156" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6">
-      <c r="A157" t="s">
-        <v>35</v>
-      </c>
-      <c r="B157">
-        <f t="shared" si="2"/>
-        <v>156</v>
-      </c>
-      <c r="C157">
-        <v>11</v>
-      </c>
-      <c r="D157" s="4">
-        <v>6</v>
-      </c>
-      <c r="E157" s="4">
-        <v>3</v>
-      </c>
-      <c r="F157" s="4">
         <v>37</v>
       </c>
     </row>
@@ -13991,6 +14019,447 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B938275A-1762-9B4D-AC4A-21F5BADA704E}">
+  <dimension ref="A1:D28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <f>AVERAGE('Master Reinforcer'!F2:F7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <f>AVERAGE('Master Reinforcer'!F50:F55)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <f>AVERAGE('Master Reinforcer'!F98:F103)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <f>AVERAGE('Master Reinforcer'!F8:F13)</f>
+        <v>174.66666666666666</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <f>AVERAGE('Master Reinforcer'!F56:F61)</f>
+        <v>3.3333333333333335</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <f>AVERAGE('Master Reinforcer'!F104:F109)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <f>AVERAGE('P4_Rosie&amp;Carlie'!C2:C7)</f>
+        <v>1.1666666666666667</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <f>AVERAGE('P4_Rosie&amp;Carlie'!D2:D7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <f>AVERAGE('P4_Rosie&amp;Carlie'!E2:E7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <f>AVERAGE('P6_Kodi &amp; Kaia'!C2:C7)</f>
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <f>AVERAGE('P6_Kodi &amp; Kaia'!D2:D7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <f>AVERAGE('P6_Kodi &amp; Kaia'!E2:E7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <f>AVERAGE('P7_Dax &amp; Fiona'!C2:C7)</f>
+        <v>204.16666666666666</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <f>AVERAGE('P7_Dax &amp; Fiona'!D2:D7)</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <f>AVERAGE('P7_Dax &amp; Fiona'!E2:E7)</f>
+        <v>105.66666666666667</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <f>AVERAGE('P8_Misha&amp;Houston'!C2:C7)</f>
+        <v>67.850000000000009</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <f>AVERAGE('P8_Misha&amp;Houston'!D2:D7)</f>
+        <v>22.75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>8</v>
+      </c>
+      <c r="D19">
+        <f>AVERAGE('P8_Misha&amp;Houston'!E2:E7)</f>
+        <v>39.416666666666664</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>9</v>
+      </c>
+      <c r="D20">
+        <f>AVERAGE('P9_Gunner&amp;Cato'!C2:C5)</f>
+        <v>135.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>9</v>
+      </c>
+      <c r="D21">
+        <f>AVERAGE('P9_Gunner&amp;Cato'!D2:D5)</f>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>9</v>
+      </c>
+      <c r="D22">
+        <f>AVERAGE('P9_Gunner&amp;Cato'!E2:E5)</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>10</v>
+      </c>
+      <c r="D23">
+        <f>AVERAGE('P10_Coffee&amp;Mason'!C2:C7)</f>
+        <v>41.833333333333336</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+      <c r="D24">
+        <f>AVERAGE('P10_Coffee&amp;Mason'!D2:D7)</f>
+        <v>7.166666666666667</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+      <c r="D25">
+        <f>AVERAGE('P10_Coffee&amp;Mason'!E2:E7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>11</v>
+      </c>
+      <c r="D26">
+        <f>AVERAGE('P11_Rev&amp;Blitz'!C2:C7)</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>11</v>
+      </c>
+      <c r="D27">
+        <f>AVERAGE('P11_Rev&amp;Blitz'!D2:D7)</f>
+        <v>13.166666666666666</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>11</v>
+      </c>
+      <c r="D28">
+        <f>AVERAGE('P11_Rev&amp;Blitz'!E2:E7)</f>
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="D2:D7" formulaRange="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -14138,7 +14607,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -14353,7 +14822,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -14645,7 +15114,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -14863,7 +15332,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -14972,7 +15441,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -15187,284 +15656,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
-  </sheetPr>
-  <dimension ref="A1:E20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="3"/>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <f>120+36+6</f>
-        <v>162</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="3"/>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <f>240+27</f>
-        <v>267</v>
-      </c>
-      <c r="D3">
-        <f>95</f>
-        <v>95</v>
-      </c>
-      <c r="E3">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="3"/>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <f>180+40+4</f>
-        <v>224</v>
-      </c>
-      <c r="D4">
-        <v>8</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="2"/>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <f>180+57</f>
-        <v>237</v>
-      </c>
-      <c r="D5">
-        <f>120+17</f>
-        <v>137</v>
-      </c>
-      <c r="E5">
-        <f>180+2</f>
-        <v>182</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="2"/>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <f>120+1+7</f>
-        <v>128</v>
-      </c>
-      <c r="D6">
-        <f>60+51+6</f>
-        <v>117</v>
-      </c>
-      <c r="E6">
-        <f>120+55</f>
-        <v>175</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="2"/>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <f>180+27</f>
-        <v>207</v>
-      </c>
-      <c r="D7">
-        <f>120+3</f>
-        <v>123</v>
-      </c>
-      <c r="E7">
-        <f>180+44</f>
-        <v>224</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="B8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8">
-        <f>SUM(C2:C7)</f>
-        <v>1225</v>
-      </c>
-      <c r="D8">
-        <f t="shared" ref="D8:E8" si="0">SUM(D2:D7)</f>
-        <v>480</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>634</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="B9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9">
-        <f>AVERAGE(C2:C7)</f>
-        <v>204.16666666666666</v>
-      </c>
-      <c r="D9">
-        <f t="shared" ref="D9:E9" si="1">AVERAGE(D2:D7)</f>
-        <v>80</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="1"/>
-        <v>105.66666666666667</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10">
-        <f>STDEV(C2:C7)</f>
-        <v>51.003594644560778</v>
-      </c>
-      <c r="D10">
-        <f t="shared" ref="D10:E10" si="2">STDEV(D2:D7)</f>
-        <v>60.4582500573743</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="2"/>
-        <v>99.740997922953767</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="B11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11">
-        <f>C10/SQRT(6)</f>
-        <v>20.822130321153779</v>
-      </c>
-      <c r="D11">
-        <f t="shared" ref="D11:E11" si="3">D10/SQRT(6)</f>
-        <v>24.681977230359809</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="3"/>
-        <v>40.719091891205593</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="C16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17">
-        <v>1225</v>
-      </c>
-      <c r="D17">
-        <v>480</v>
-      </c>
-      <c r="E17">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18">
-        <v>204.16666666666666</v>
-      </c>
-      <c r="D18">
-        <v>80</v>
-      </c>
-      <c r="E18">
-        <v>105.66666666666667</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19">
-        <v>51.003594644560778</v>
-      </c>
-      <c r="D19">
-        <v>60.4582500573743</v>
-      </c>
-      <c r="E19">
-        <v>99.740997922953767</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20">
-        <v>20.822130321153779</v>
-      </c>
-      <c r="D20">
-        <v>24.681977230359809</v>
-      </c>
-      <c r="E20">
-        <v>40.719091891205593</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>